<commit_message>
modified:   tutorial/supply/excel_reader.py 	modified:   tutorial/supply/exceltemplate.ini 	modified:   tutorial/supply/main.py
</commit_message>
<xml_diff>
--- a/tutorial/supply/供应商数据表/安全钳数据表.xlsx
+++ b/tutorial/supply/供应商数据表/安全钳数据表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chengzhenbo/Library/Mobile Documents/com~apple~CloudDocs/04Project/ElevatorCertificate/ElevatorCertificate/tutorial/supply/供应商数据表/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD6B086-7662-6146-A511-1C8E27624B93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0386944-4130-0945-9B00-FD19E816566A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6120" yWindow="460" windowWidth="27840" windowHeight="16940" xr2:uid="{4097CB3E-8DF1-364E-9180-12105D07802D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>安全钳</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -109,6 +109,38 @@
   </si>
   <si>
     <t>2020.1.9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -758,7 +790,7 @@
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3"/>
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -861,11 +893,21 @@
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="F3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="K3" s="3" t="s">
         <v>18</v>
       </c>
@@ -875,11 +917,19 @@
       <c r="M3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
+      <c r="N3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="O3" s="5">
+        <v>2</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
+      <c r="R3" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="S3" s="5" t="s">
         <v>19</v>
       </c>

</xml_diff>